<commit_message>
can't write to stocks_records wb for some reason, taking a break
</commit_message>
<xml_diff>
--- a/Stock_Records.xlsx
+++ b/Stock_Records.xlsx
@@ -2,35 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2be85617f88dbbd4/Documents/Git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2be85617f88dbbd4/Documents/PythonProjects/Git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08754506-1326-498A-B49C-7593EF0F3463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{7955D20B-092A-4980-B95D-A5C4D62B3E43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F05D58B-C7DF-4B04-8805-EFE550C810C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>0</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -71,7 +65,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -94,44 +88,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -158,32 +152,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -210,24 +186,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -239,153 +197,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC06F62-71CD-4FB2-9493-84EB23AEA023}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished stock_puller, stock_excel currently ads the current date to the work sheet. need it to create a new sheet every time and then add entered stocks and their scraped prices to the new sheet
</commit_message>
<xml_diff>
--- a/Stock_Records.xlsx
+++ b/Stock_Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2be85617f88dbbd4/Documents/PythonProjects/Git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{7955D20B-092A-4980-B95D-A5C4D62B3E43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{FA5DCB15-1D0F-4695-8D4A-3D471B21DD1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>0</t>
+    <t>12/20/20</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Stocks_Excel.py now works using trial lists
</commit_message>
<xml_diff>
--- a/Stock_Records.xlsx
+++ b/Stock_Records.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3150" yWindow="1500" windowWidth="21600" windowHeight="11715" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet6" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -412,9 +413,80 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>01/04/21</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>stock1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>stock2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>stock3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>stock4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>stock5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -423,7 +495,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>12/28/20</t>
+          <t>01/04/21</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>stock1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>price1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>stock2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>price2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>stock3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>price3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>stock4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>price4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>stock5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>price5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
program now takes stock tickers as an argument and collects their current price. Enters date into cell A1 and enters lists of tickers and list of stock prices into the excel file on a new page each time. Problem: adds whatever you used to break the loop to the list as well
</commit_message>
<xml_diff>
--- a/Stock_Records.xlsx
+++ b/Stock_Records.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3150" yWindow="1500" windowWidth="21600" windowHeight="11715" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2880" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet6" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet7" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet8" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -413,10 +414,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -424,7 +425,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>01/04/21</t>
+          <t>01/05/21</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -435,41 +436,6 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>stock1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>stock2</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>stock3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>stock4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>stock5</t>
         </is>
       </c>
     </row>
@@ -486,6 +452,102 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>01/12/21</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>stock1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>price1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>stock2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>price2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>stock3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>price3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>stock4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>price4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>stock5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>price5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -495,7 +557,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>01/04/21</t>
+          <t>01/12/21</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -512,60 +574,43 @@
     <row r="2">
       <c r="C2" t="inlineStr">
         <is>
-          <t>stock1</t>
+          <t>tsla</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>price1</t>
+          <t>849.44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="C3" t="inlineStr">
         <is>
-          <t>stock2</t>
+          <t>ge</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>price2</t>
+          <t>11.78</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="C4" t="inlineStr">
         <is>
-          <t>stock3</t>
+          <t>gme</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>price3</t>
+          <t>19.95</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>stock4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>price4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>stock5</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>price5</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>